<commit_message>
Smoke and regression tags
</commit_message>
<xml_diff>
--- a/src/test/resources/com/travelocity/test-data/1.xlsx
+++ b/src/test/resources/com/travelocity/test-data/1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0CEF5B95-96E3-43B0-B304-12E588650852}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{1094EEAD-C56D-4BE3-9878-3488CAA277B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="20790" windowHeight="11820" xr2:uid="{FE8D01E6-C1E3-4338-AC3B-B82F2337A162}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="20790" windowHeight="11820" xr2:uid="{FE8D01E6-C1E3-4338-AC3B-B82F2337A162}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -457,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E752E530-4C12-4F61-B562-BFFFB21CE8A8}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,16 +547,12 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E5" s="1"/>
-    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>